<commit_message>
Metode til beregning af startværdier påbegyndt.
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/Othdata_dors_2.xlsx
+++ b/examples/Abatement/Data/Othdata_dors_2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\GPM_v05\examples\Abatement\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zgr679\Documents\GitHub\GPM_v05\examples\Abatement\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>mu/n</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>qS/n</t>
+  </si>
+  <si>
+    <t>qS/qS</t>
   </si>
 </sst>
 </file>
@@ -416,13 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +446,14 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -455,8 +469,14 @@
       <c r="E2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -473,7 +493,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -484,7 +504,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -495,7 +515,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -506,7 +526,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -527,7 +547,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +683,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Lavede sidste merge forkert stupid me
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/Othdata_dors_2.xlsx
+++ b/examples/Abatement/Data/Othdata_dors_2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\GPM_v05\examples\Abatement\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zgr679\Documents\GitHub\GPM_v05\examples\Abatement\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>mu/n</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>qS/n</t>
+  </si>
+  <si>
+    <t>qS/qS</t>
   </si>
 </sst>
 </file>
@@ -416,13 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +446,14 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -455,8 +469,14 @@
       <c r="E2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -473,7 +493,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -484,7 +504,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -495,7 +515,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -506,7 +526,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -581,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add_sets henter nu også lidt mere fra output/tech (kataloget)
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/Othdata_dors_2.xlsx
+++ b/examples/Abatement/Data/Othdata_dors_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mere konsistente priser, høj sigma + stigende CO2-pris. simuleringer
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/Othdata_dors_2.xlsx
+++ b/examples/Abatement/Data/Othdata_dors_2.xlsx
@@ -602,7 +602,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
         <v>19</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>

</xml_diff>